<commit_message>
04/07- Enhancing the keyword framework to support multi tabs in sheet
</commit_message>
<xml_diff>
--- a/HubSpot_TestData.xlsx
+++ b/HubSpot_TestData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Signup" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>test step</t>
   </si>
   <si>
-    <t>locator</t>
-  </si>
-  <si>
     <t xml:space="preserve">action </t>
   </si>
   <si>
@@ -59,9 +57,6 @@
     <t>enter email address</t>
   </si>
   <si>
-    <t>id=username</t>
-  </si>
-  <si>
     <t>sendkeys</t>
   </si>
   <si>
@@ -71,18 +66,12 @@
     <t>enter password</t>
   </si>
   <si>
-    <t>id=password</t>
-  </si>
-  <si>
     <t>Test@123</t>
   </si>
   <si>
     <t>click on login button</t>
   </si>
   <si>
-    <t>id=loginBtn</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -95,7 +84,28 @@
     <t>verify sign up link</t>
   </si>
   <si>
-    <t>linkText=Sign up</t>
+    <t>locatorType</t>
+  </si>
+  <si>
+    <t>locatorValue</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>loginBtn</t>
+  </si>
+  <si>
+    <t>linkText</t>
+  </si>
+  <si>
+    <t>Sign up</t>
   </si>
 </sst>
 </file>
@@ -438,182 +448,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="2" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
+      <c r="E5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
04/07- Enhancing the keyword framework to support multi tabs in sheet Part 2
</commit_message>
<xml_diff>
--- a/HubSpot_TestData.xlsx
+++ b/HubSpot_TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>test step</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Sign up</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>